<commit_message>
edit remove, serch function. Regenerate Tests Results
</commit_message>
<xml_diff>
--- a/semestrovka2/testsResult/InsertTest.xlsx
+++ b/semestrovka2/testsResult/InsertTest.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,22 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projectjava\Alg&amp;DataStr\sem2\testsResult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5E959D7-34A6-4488-8EDE-18B821827ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEE73F4C-117A-42A7-8C1C-6BB847D37C42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2184" yWindow="3696" windowWidth="17280" windowHeight="9960"/>
   </bookViews>
   <sheets>
     <sheet name="InsertTest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -48,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -907,11 +899,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,21 +924,23 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3324106</v>
+        <v>17403600</v>
       </c>
       <c r="B2">
         <v>544732</v>
       </c>
       <c r="E2">
-        <v>1090657.1200000001</v>
+        <f>AVERAGE(A2:A51)</f>
+        <v>3449470</v>
       </c>
       <c r="F2">
+        <f>AVERAGE(B2:B51)</f>
         <v>544732</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2167991</v>
+        <v>12462300</v>
       </c>
       <c r="B3">
         <v>544732</v>
@@ -957,21 +951,23 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1406189</v>
+        <v>1357300</v>
       </c>
       <c r="B4">
         <v>544732</v>
       </c>
       <c r="E4" s="1">
-        <v>109.065712</v>
+        <f>E2/10000</f>
+        <v>344.947</v>
       </c>
       <c r="F4" s="1">
+        <f>F2/10000</f>
         <v>54.473199999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1362098</v>
+        <v>2256200</v>
       </c>
       <c r="B5">
         <v>544732</v>
@@ -979,7 +975,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1137412</v>
+        <v>1238000</v>
       </c>
       <c r="B6">
         <v>544732</v>
@@ -987,7 +983,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1106411</v>
+        <v>1308200</v>
       </c>
       <c r="B7">
         <v>544732</v>
@@ -995,7 +991,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1124981</v>
+        <v>1259400</v>
       </c>
       <c r="B8">
         <v>544732</v>
@@ -1003,7 +999,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1146394</v>
+        <v>1097800</v>
       </c>
       <c r="B9">
         <v>544732</v>
@@ -1011,7 +1007,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1030091</v>
+        <v>1520300</v>
       </c>
       <c r="B10">
         <v>544732</v>
@@ -1019,7 +1015,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>919791</v>
+        <v>5142600</v>
       </c>
       <c r="B11">
         <v>544732</v>
@@ -1027,7 +1023,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>951912</v>
+        <v>10183100</v>
       </c>
       <c r="B12">
         <v>544732</v>
@@ -1035,7 +1031,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>911011</v>
+        <v>3272200</v>
       </c>
       <c r="B13">
         <v>544732</v>
@@ -1043,7 +1039,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>946716</v>
+        <v>7062100</v>
       </c>
       <c r="B14">
         <v>544732</v>
@@ -1051,7 +1047,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>880301</v>
+        <v>8844100</v>
       </c>
       <c r="B15">
         <v>544732</v>
@@ -1059,7 +1055,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>882917</v>
+        <v>4281200</v>
       </c>
       <c r="B16">
         <v>544732</v>
@@ -1067,7 +1063,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>863192</v>
+        <v>3002000</v>
       </c>
       <c r="B17">
         <v>544732</v>
@@ -1075,7 +1071,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>965391</v>
+        <v>1329300</v>
       </c>
       <c r="B18">
         <v>544732</v>
@@ -1083,7 +1079,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>1116708</v>
+        <v>2981000</v>
       </c>
       <c r="B19">
         <v>544732</v>
@@ -1091,7 +1087,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1098794</v>
+        <v>10080000</v>
       </c>
       <c r="B20">
         <v>544732</v>
@@ -1099,7 +1095,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>1101497</v>
+        <v>6896100</v>
       </c>
       <c r="B21">
         <v>544732</v>
@@ -1107,7 +1103,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>1170217</v>
+        <v>1118000</v>
       </c>
       <c r="B22">
         <v>544732</v>
@@ -1115,7 +1111,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>1193924</v>
+        <v>1167200</v>
       </c>
       <c r="B23">
         <v>544732</v>
@@ -1123,7 +1119,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>1147007</v>
+        <v>1215800</v>
       </c>
       <c r="B24">
         <v>544732</v>
@@ -1131,7 +1127,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>1234786</v>
+        <v>1132600</v>
       </c>
       <c r="B25">
         <v>544732</v>
@@ -1139,7 +1135,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>1110288</v>
+        <v>11329600</v>
       </c>
       <c r="B26">
         <v>544732</v>
@@ -1147,7 +1143,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>945512</v>
+        <v>7597300</v>
       </c>
       <c r="B27">
         <v>544732</v>
@@ -1155,7 +1151,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>905194</v>
+        <v>6707200</v>
       </c>
       <c r="B28">
         <v>544732</v>
@@ -1163,7 +1159,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>889201</v>
+        <v>1600500</v>
       </c>
       <c r="B29">
         <v>544732</v>
@@ -1171,7 +1167,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>896805</v>
+        <v>6063900</v>
       </c>
       <c r="B30">
         <v>544732</v>
@@ -1179,7 +1175,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>877707</v>
+        <v>885600</v>
       </c>
       <c r="B31">
         <v>544732</v>
@@ -1187,7 +1183,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>869210</v>
+        <v>896700</v>
       </c>
       <c r="B32">
         <v>544732</v>
@@ -1195,7 +1191,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>881413</v>
+        <v>7938700</v>
       </c>
       <c r="B33">
         <v>544732</v>
@@ -1203,7 +1199,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>895712</v>
+        <v>903400</v>
       </c>
       <c r="B34">
         <v>544732</v>
@@ -1211,7 +1207,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>890696</v>
+        <v>1135100</v>
       </c>
       <c r="B35">
         <v>544732</v>
@@ -1219,7 +1215,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>862302</v>
+        <v>858400</v>
       </c>
       <c r="B36">
         <v>544732</v>
@@ -1227,7 +1223,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>906698</v>
+        <v>901800</v>
       </c>
       <c r="B37">
         <v>544732</v>
@@ -1235,7 +1231,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>950101</v>
+        <v>889100</v>
       </c>
       <c r="B38">
         <v>544732</v>
@@ -1243,7 +1239,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>1309593</v>
+        <v>879200</v>
       </c>
       <c r="B39">
         <v>544732</v>
@@ -1251,7 +1247,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>892092</v>
+        <v>871600</v>
       </c>
       <c r="B40">
         <v>544732</v>
@@ -1259,7 +1255,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>871285</v>
+        <v>889500</v>
       </c>
       <c r="B41">
         <v>544732</v>
@@ -1267,7 +1263,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>884089</v>
+        <v>908400</v>
       </c>
       <c r="B42">
         <v>544732</v>
@@ -1275,7 +1271,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>889901</v>
+        <v>875400</v>
       </c>
       <c r="B43">
         <v>544732</v>
@@ -1283,7 +1279,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>865898</v>
+        <v>874400</v>
       </c>
       <c r="B44">
         <v>544732</v>
@@ -1291,7 +1287,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>860601</v>
+        <v>1086700</v>
       </c>
       <c r="B45">
         <v>544732</v>
@@ -1299,7 +1295,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>1123510</v>
+        <v>1123000</v>
       </c>
       <c r="B46">
         <v>544732</v>
@@ -1307,7 +1303,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>1132910</v>
+        <v>3740200</v>
       </c>
       <c r="B47">
         <v>544732</v>
@@ -1315,7 +1311,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1258306</v>
+        <v>1452000</v>
       </c>
       <c r="B48">
         <v>544732</v>
@@ -1323,7 +1319,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>1095208</v>
+        <v>1528600</v>
       </c>
       <c r="B49">
         <v>544732</v>
@@ -1331,7 +1327,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>1146683</v>
+        <v>1374700</v>
       </c>
       <c r="B50">
         <v>544732</v>
@@ -1339,7 +1335,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>1132104</v>
+        <v>1552100</v>
       </c>
       <c r="B51">
         <v>544732</v>

</xml_diff>